<commit_message>
feat: renamed 'mappedBy' to more understable 'refBack'
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-semantics/src/test/resources/fdp.xlsx
+++ b/backend/molgenis-emx2-semantics/src/test/resources/fdp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-semantics/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753E4306-387D-CA40-97C1-2FB9A2F00943}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7F3F21-9019-5348-9FF0-316AC16F8F42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{FC3106C0-1D46-C24B-9B5F-C0729D326D4C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{FC3106C0-1D46-C24B-9B5F-C0729D326D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,6 @@
     <t>catalogIdentifier</t>
   </si>
   <si>
-    <t>mappedBy</t>
-  </si>
-  <si>
     <t>2020-09-22T22:22</t>
   </si>
   <si>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>semantics</t>
+  </si>
+  <si>
+    <t>refBack</t>
   </si>
 </sst>
 </file>
@@ -637,7 +637,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -667,29 +667,29 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>14</v>
@@ -701,12 +701,12 @@
         <v>1</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>6</v>
@@ -718,12 +718,12 @@
         <v>2</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>5</v>
@@ -732,12 +732,12 @@
         <v>16</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>7</v>
@@ -746,12 +746,12 @@
         <v>9</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>8</v>
@@ -760,12 +760,12 @@
         <v>15</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>17</v>
@@ -780,12 +780,12 @@
         <v>19</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>10</v>
@@ -794,12 +794,12 @@
         <v>12</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>11</v>
@@ -808,7 +808,7 @@
         <v>12</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -816,7 +816,7 @@
         <v>13</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="13" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -833,7 +833,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="13" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -847,10 +847,10 @@
         <v>4</v>
       </c>
       <c r="E13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -867,7 +867,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -881,7 +881,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -895,7 +895,7 @@
         <v>9</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -909,7 +909,7 @@
         <v>15</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -923,7 +923,7 @@
         <v>12</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -937,7 +937,7 @@
         <v>12</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -993,7 +993,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -1008,10 +1008,10 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1071,16 +1071,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="6">
         <v>1</v>
@@ -1089,24 +1089,24 @@
         <v>23</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="6">
         <v>1</v>
@@ -1115,10 +1115,10 @@
         <v>23</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>